<commit_message>
updated visualisation app. 50% completed
</commit_message>
<xml_diff>
--- a/data/growth.xlsx
+++ b/data/growth.xlsx
@@ -482,19 +482,19 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.2159</v>
+        <v>0.2158</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1.5285</v>
+        <v>1.5279</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>-0.1706</v>
+        <v>-0.1704</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>26.8549</v>
+        <v>11.2932</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>-4.1022</v>
+        <v>-8.7913</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>-0.7246</v>

</xml_diff>